<commit_message>
penambahan preprocessing data buku, dan perepresentasian dari data sirkulasi ke data matriks frekuensi yang siap olah untuk input CF
</commit_message>
<xml_diff>
--- a/datatoybuku.xlsx
+++ b/datatoybuku.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Universitas Trunojoyo Madura\#Kuliah\#SKRIPSI\dokumen\program\sv-k-modes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D4DF64-7A08-43AF-A6F0-B81A57182842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7FAE3DB-2B47-4496-A8F2-B4A7D8D3663D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F4C2F87C-C899-4D8E-B337-531C6F58FF5C}"/>
   </bookViews>
@@ -38,38 +38,46 @@
     <t>manusia, salmon</t>
   </si>
   <si>
-    <t>kepemimpinan, organisasi</t>
-  </si>
-  <si>
-    <t>corel draw</t>
-  </si>
-  <si>
-    <t>ekonomi</t>
-  </si>
-  <si>
-    <t>ekonomi, mikro</t>
-  </si>
-  <si>
     <t>ekonomi, moneter</t>
   </si>
   <si>
     <t>sekolah, jaringan</t>
   </si>
   <si>
-    <t>kepemimpinan, sekolah, budaya mutu</t>
-  </si>
-  <si>
     <t>komunikasi, manusia</t>
+  </si>
+  <si>
+    <t>ekonomi, MiKro</t>
+  </si>
+  <si>
+    <t>kepemimpinan; organisasi</t>
+  </si>
+  <si>
+    <t>corel-draw12</t>
+  </si>
+  <si>
+    <t>ekonomi!@##</t>
+  </si>
+  <si>
+    <t>kepemimpinan, SEkolah, budaya     mutu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,13 +100,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,7 +425,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,7 +439,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,8 +454,8 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -460,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -476,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -484,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -492,10 +503,13 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{67B02B64-A018-48C9-9591-9B73529B6650}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>